<commit_message>
Nouveaux Tarifs et bon de commande.
Update du bon de commande et des tarifs.
</commit_message>
<xml_diff>
--- a/assets/Bon_de_commande_THETYS.xlsx
+++ b/assets/Bon_de_commande_THETYS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinpuy/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7F74C12-A3A4-C344-96ED-44C88E793C71}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5C9BA-A734-654B-9FB3-C19FEA26DA26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="27600" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -232,7 +232,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -267,6 +267,12 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
     <fill>
@@ -400,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -436,10 +442,10 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -459,6 +465,8 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -723,8 +731,8 @@
   </sheetPr>
   <dimension ref="A1:AE440"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="115" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="134" workbookViewId="0">
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1299,10 +1307,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="13"/>
-      <c r="E26" s="7" t="s">
+      <c r="E26" s="40" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="6">
+      <c r="F26" s="41">
         <v>0</v>
       </c>
       <c r="G26"/>
@@ -1317,10 +1325,10 @@
     </row>
     <row r="27" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="20"/>
-      <c r="B27" s="27" t="s">
+      <c r="B27" s="29" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="28">
+      <c r="C27" s="30">
         <v>0</v>
       </c>
       <c r="D27"/>
@@ -1424,10 +1432,10 @@
       <c r="AD31" s="16"/>
     </row>
     <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="30" t="s">
+      <c r="A32" s="28" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="29"/>
+      <c r="B32" s="27"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>

</xml_diff>

<commit_message>
Correction update Bon de commande.
modification du bon de commande qui a mal été updaté.
</commit_message>
<xml_diff>
--- a/assets/Bon_de_commande_THETYS.xlsx
+++ b/assets/Bon_de_commande_THETYS.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinpuy/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FF5C9BA-A734-654B-9FB3-C19FEA26DA26}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7615901-EE2D-3241-9671-92D99EF01CEE}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="460" windowWidth="27600" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1240" yWindow="460" windowWidth="27560" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuille 1" sheetId="1" r:id="rId1"/>
@@ -406,7 +406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -430,14 +430,8 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -450,23 +444,33 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" xfId="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
@@ -731,8 +735,8 @@
   </sheetPr>
   <dimension ref="A1:AE440"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A3" zoomScale="134" workbookViewId="0">
-      <selection activeCell="G30" sqref="G30"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A5" zoomScale="134" workbookViewId="0">
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -754,456 +758,761 @@
     <col min="31" max="16384" width="14.5" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="20"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="34"/>
-      <c r="D1" s="34"/>
-      <c r="E1" s="34"/>
-      <c r="F1" s="34"/>
+    <row r="1" spans="1:31" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17"/>
+      <c r="B1" s="37"/>
+      <c r="C1" s="32"/>
+      <c r="D1" s="32"/>
+      <c r="E1" s="32"/>
+      <c r="F1" s="32"/>
       <c r="G1"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="32"/>
-      <c r="J1" s="32"/>
-      <c r="K1" s="32"/>
-      <c r="L1" s="31"/>
-      <c r="M1" s="32"/>
-      <c r="N1" s="32"/>
-      <c r="O1" s="32"/>
-      <c r="P1" s="22"/>
-      <c r="Q1" s="22"/>
-      <c r="R1" s="22"/>
-    </row>
-    <row r="2" spans="1:31" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="21"/>
-      <c r="B2" s="34"/>
-      <c r="C2" s="34"/>
-      <c r="D2" s="34"/>
-      <c r="E2" s="34"/>
-      <c r="F2" s="34"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="35"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="27"/>
+      <c r="R1" s="27"/>
+      <c r="S1" s="28"/>
+      <c r="T1" s="28"/>
+      <c r="U1" s="28"/>
+      <c r="V1" s="28"/>
+      <c r="W1" s="28"/>
+      <c r="X1" s="28"/>
+      <c r="Y1" s="28"/>
+      <c r="Z1" s="28"/>
+      <c r="AA1" s="28"/>
+      <c r="AB1" s="28"/>
+      <c r="AC1" s="28"/>
+      <c r="AD1" s="28"/>
+    </row>
+    <row r="2" spans="1:31" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A2" s="18"/>
+      <c r="B2" s="32"/>
+      <c r="C2" s="32"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
       <c r="G2"/>
-      <c r="P2" s="24" t="s">
+      <c r="H2" s="28"/>
+      <c r="I2" s="28"/>
+      <c r="J2" s="28"/>
+      <c r="K2" s="28"/>
+      <c r="L2" s="28"/>
+      <c r="M2" s="28"/>
+      <c r="N2" s="28"/>
+      <c r="O2" s="28"/>
+      <c r="P2" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="23" t="s">
+      <c r="Q2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="24" t="s">
+      <c r="R2" s="20" t="s">
         <v>2</v>
       </c>
-      <c r="S2" s="23" t="s">
+      <c r="S2" s="28" t="s">
         <v>3</v>
       </c>
-      <c r="T2" s="23" t="s">
+      <c r="T2" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="V2" s="25"/>
-      <c r="W2" s="23" t="s">
+      <c r="U2" s="28"/>
+      <c r="V2" s="21"/>
+      <c r="W2" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="X2" s="23" t="s">
+      <c r="X2" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="Y2" s="23" t="s">
+      <c r="Y2" s="28" t="s">
         <v>7</v>
       </c>
-      <c r="Z2" s="23" t="s">
+      <c r="Z2" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="AA2" s="24" t="s">
+      <c r="AA2" s="20" t="s">
         <v>9</v>
       </c>
-      <c r="AB2" s="24" t="s">
+      <c r="AB2" s="20" t="s">
         <v>10</v>
       </c>
-      <c r="AC2" s="24" t="s">
+      <c r="AC2" s="20" t="s">
         <v>11</v>
       </c>
-      <c r="AD2" s="24" t="s">
+      <c r="AD2" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="25"/>
-    </row>
-    <row r="3" spans="1:31" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="21"/>
-      <c r="B3" s="34"/>
-      <c r="C3" s="34"/>
-      <c r="D3" s="34"/>
-      <c r="E3" s="34"/>
-      <c r="F3" s="34"/>
+      <c r="AE2" s="21"/>
+    </row>
+    <row r="3" spans="1:31" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="18"/>
+      <c r="B3" s="32"/>
+      <c r="C3" s="32"/>
+      <c r="D3" s="32"/>
+      <c r="E3" s="32"/>
+      <c r="F3" s="32"/>
       <c r="G3"/>
-      <c r="P3" s="26">
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="22">
         <f>R3+T3+G3</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="25">
+      <c r="Q3" s="21">
         <f>SUM(H3:K3)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="25">
-        <f>24*2.5*X3+6*2.8333333333*Z3+Y3*3.2</f>
+      <c r="R3" s="21">
+        <f>24*2.5*X3+6*2.8333333333*Z3+Y3*3.3</f>
         <v>0</v>
       </c>
-      <c r="S3" s="25">
+      <c r="S3" s="21">
         <f>SUM(L3:O3)</f>
         <v>0</v>
       </c>
-      <c r="T3" s="25">
+      <c r="T3" s="21">
         <f>6*5*AB3+3*5.8333333333*AD3+AC3*6.8</f>
         <v>0</v>
       </c>
-      <c r="U3" s="25"/>
-      <c r="V3" s="25"/>
-      <c r="W3" s="25">
+      <c r="U3" s="21"/>
+      <c r="V3" s="21"/>
+      <c r="W3" s="21">
         <f>MOD(C28,24)</f>
         <v>0</v>
       </c>
-      <c r="X3" s="25">
+      <c r="X3" s="21">
         <f>QUOTIENT(C28,24)</f>
         <v>0</v>
       </c>
-      <c r="Y3" s="25">
+      <c r="Y3" s="21">
         <f>MOD(C28-24*W3,6)</f>
         <v>0</v>
       </c>
-      <c r="Z3" s="25">
+      <c r="Z3" s="21">
         <f>QUOTIENT(C28-24*X3,6)</f>
         <v>0</v>
       </c>
-      <c r="AA3" s="26">
+      <c r="AA3" s="22">
         <f>MOD(F28,6)</f>
         <v>0</v>
       </c>
-      <c r="AB3" s="26">
+      <c r="AB3" s="22">
         <f>QUOTIENT(F28,6)</f>
         <v>0</v>
       </c>
-      <c r="AC3" s="26">
+      <c r="AC3" s="22">
         <f>MOD(F28-6*AB3,3)</f>
         <v>0</v>
       </c>
-      <c r="AD3" s="26">
+      <c r="AD3" s="22">
         <f>QUOTIENT(F28-6*AB3,3)</f>
         <v>0</v>
       </c>
-      <c r="AE3" s="25"/>
-    </row>
-    <row r="4" spans="1:31" s="23" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="20"/>
-      <c r="B4" s="34"/>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
+      <c r="AE3" s="21"/>
+    </row>
+    <row r="4" spans="1:31" s="19" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A4" s="17"/>
+      <c r="B4" s="32"/>
+      <c r="C4" s="32"/>
+      <c r="D4" s="32"/>
+      <c r="E4" s="32"/>
+      <c r="F4" s="32"/>
       <c r="G4"/>
-      <c r="P4" s="26"/>
-      <c r="AA4" s="26"/>
-      <c r="AB4" s="26"/>
-      <c r="AC4" s="26"/>
-      <c r="AD4" s="26"/>
+      <c r="H4" s="28"/>
+      <c r="I4" s="28"/>
+      <c r="J4" s="28"/>
+      <c r="K4" s="28"/>
+      <c r="L4" s="28"/>
+      <c r="M4" s="28"/>
+      <c r="N4" s="28"/>
+      <c r="O4" s="28"/>
+      <c r="P4" s="22"/>
+      <c r="Q4" s="28"/>
+      <c r="R4" s="28"/>
+      <c r="S4" s="28"/>
+      <c r="T4" s="28"/>
+      <c r="U4" s="28"/>
+      <c r="V4" s="28"/>
+      <c r="W4" s="28"/>
+      <c r="X4" s="28"/>
+      <c r="Y4" s="28"/>
+      <c r="Z4" s="28"/>
+      <c r="AA4" s="22"/>
+      <c r="AB4" s="22"/>
+      <c r="AC4" s="22"/>
+      <c r="AD4" s="22"/>
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A5" s="20"/>
-      <c r="B5" s="34"/>
-      <c r="C5" s="34"/>
-      <c r="D5" s="34"/>
-      <c r="E5" s="34"/>
-      <c r="F5" s="34"/>
+      <c r="A5" s="17"/>
+      <c r="B5" s="32"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="32"/>
+      <c r="F5" s="32"/>
       <c r="G5"/>
-      <c r="H5" s="15"/>
-      <c r="L5" s="15"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="16"/>
-      <c r="AA5" s="16"/>
-      <c r="AB5" s="16"/>
-      <c r="AC5" s="16"/>
-      <c r="AD5" s="16"/>
+      <c r="H5" s="40"/>
+      <c r="I5" s="41"/>
+      <c r="J5" s="41"/>
+      <c r="K5" s="41"/>
+      <c r="L5" s="40"/>
+      <c r="M5" s="41"/>
+      <c r="N5" s="41"/>
+      <c r="O5" s="40"/>
+      <c r="P5" s="42"/>
+      <c r="Q5" s="41"/>
+      <c r="R5" s="41"/>
+      <c r="S5" s="41"/>
+      <c r="T5" s="41"/>
+      <c r="U5" s="41"/>
+      <c r="V5" s="41"/>
+      <c r="W5" s="41"/>
+      <c r="X5" s="41"/>
+      <c r="Y5" s="41"/>
+      <c r="Z5" s="41"/>
+      <c r="AA5" s="42"/>
+      <c r="AB5" s="42"/>
+      <c r="AC5" s="42"/>
+      <c r="AD5" s="42"/>
     </row>
     <row r="6" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="20"/>
+      <c r="A6" s="17"/>
       <c r="B6"/>
       <c r="C6"/>
       <c r="D6"/>
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6"/>
-      <c r="H6" s="15"/>
-      <c r="L6" s="15"/>
-      <c r="O6" s="15"/>
-      <c r="P6" s="16"/>
-      <c r="AA6" s="16"/>
-      <c r="AB6" s="16"/>
-      <c r="AC6" s="16"/>
-      <c r="AD6" s="16"/>
+      <c r="H6" s="40"/>
+      <c r="I6" s="41"/>
+      <c r="J6" s="41"/>
+      <c r="K6" s="41"/>
+      <c r="L6" s="40"/>
+      <c r="M6" s="41"/>
+      <c r="N6" s="41"/>
+      <c r="O6" s="40"/>
+      <c r="P6" s="42"/>
+      <c r="Q6" s="41"/>
+      <c r="R6" s="41"/>
+      <c r="S6" s="41"/>
+      <c r="T6" s="41"/>
+      <c r="U6" s="41"/>
+      <c r="V6" s="41"/>
+      <c r="W6" s="41"/>
+      <c r="X6" s="41"/>
+      <c r="Y6" s="41"/>
+      <c r="Z6" s="41"/>
+      <c r="AA6" s="42"/>
+      <c r="AB6" s="42"/>
+      <c r="AC6" s="42"/>
+      <c r="AD6" s="42"/>
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="20"/>
+      <c r="A7" s="17"/>
       <c r="B7"/>
       <c r="C7"/>
       <c r="D7"/>
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7"/>
-      <c r="H7" s="15"/>
-      <c r="L7" s="15"/>
-      <c r="O7" s="15"/>
-      <c r="P7" s="16"/>
-      <c r="AA7" s="16"/>
-      <c r="AB7" s="16"/>
-      <c r="AC7" s="16"/>
-      <c r="AD7" s="16"/>
+      <c r="H7" s="40"/>
+      <c r="I7" s="41"/>
+      <c r="J7" s="41"/>
+      <c r="K7" s="41"/>
+      <c r="L7" s="40"/>
+      <c r="M7" s="41"/>
+      <c r="N7" s="41"/>
+      <c r="O7" s="40"/>
+      <c r="P7" s="42"/>
+      <c r="Q7" s="41"/>
+      <c r="R7" s="41"/>
+      <c r="S7" s="41"/>
+      <c r="T7" s="41"/>
+      <c r="U7" s="41"/>
+      <c r="V7" s="41"/>
+      <c r="W7" s="41"/>
+      <c r="X7" s="41"/>
+      <c r="Y7" s="41"/>
+      <c r="Z7" s="41"/>
+      <c r="AA7" s="42"/>
+      <c r="AB7" s="42"/>
+      <c r="AC7" s="42"/>
+      <c r="AD7" s="42"/>
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="20"/>
+      <c r="A8" s="17"/>
       <c r="B8"/>
       <c r="C8"/>
       <c r="D8"/>
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8"/>
-      <c r="H8" s="15"/>
-      <c r="L8" s="15"/>
-      <c r="O8" s="15"/>
-      <c r="P8" s="16"/>
-      <c r="AA8" s="16"/>
-      <c r="AB8" s="16"/>
-      <c r="AC8" s="16"/>
-      <c r="AD8" s="16"/>
+      <c r="H8" s="40"/>
+      <c r="I8" s="41"/>
+      <c r="J8" s="41"/>
+      <c r="K8" s="41"/>
+      <c r="L8" s="40"/>
+      <c r="M8" s="41"/>
+      <c r="N8" s="41"/>
+      <c r="O8" s="40"/>
+      <c r="P8" s="42"/>
+      <c r="Q8" s="41"/>
+      <c r="R8" s="41"/>
+      <c r="S8" s="41"/>
+      <c r="T8" s="41"/>
+      <c r="U8" s="41"/>
+      <c r="V8" s="41"/>
+      <c r="W8" s="41"/>
+      <c r="X8" s="41"/>
+      <c r="Y8" s="41"/>
+      <c r="Z8" s="41"/>
+      <c r="AA8" s="42"/>
+      <c r="AB8" s="42"/>
+      <c r="AC8" s="42"/>
+      <c r="AD8" s="42"/>
     </row>
     <row r="9" spans="1:31" ht="20" x14ac:dyDescent="0.2">
-      <c r="A9" s="20"/>
-      <c r="B9" s="35" t="s">
+      <c r="A9" s="17"/>
+      <c r="B9" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="36"/>
-      <c r="D9" s="36"/>
-      <c r="E9" s="36"/>
-      <c r="F9" s="36"/>
+      <c r="C9" s="39"/>
+      <c r="D9" s="39"/>
+      <c r="E9" s="39"/>
+      <c r="F9" s="39"/>
       <c r="G9"/>
-      <c r="H9" s="15"/>
-      <c r="L9" s="15"/>
-      <c r="O9" s="15"/>
-      <c r="P9" s="16"/>
-      <c r="AA9" s="16"/>
-      <c r="AB9" s="16"/>
-      <c r="AC9" s="16"/>
-      <c r="AD9" s="16"/>
+      <c r="H9" s="40"/>
+      <c r="I9" s="41"/>
+      <c r="J9" s="41"/>
+      <c r="K9" s="41"/>
+      <c r="L9" s="40"/>
+      <c r="M9" s="41"/>
+      <c r="N9" s="41"/>
+      <c r="O9" s="40"/>
+      <c r="P9" s="42"/>
+      <c r="Q9" s="41"/>
+      <c r="R9" s="41"/>
+      <c r="S9" s="41"/>
+      <c r="T9" s="41"/>
+      <c r="U9" s="41"/>
+      <c r="V9" s="41"/>
+      <c r="W9" s="41"/>
+      <c r="X9" s="41"/>
+      <c r="Y9" s="41"/>
+      <c r="Z9" s="41"/>
+      <c r="AA9" s="42"/>
+      <c r="AB9" s="42"/>
+      <c r="AC9" s="42"/>
+      <c r="AD9" s="42"/>
     </row>
     <row r="10" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A10" s="20"/>
+      <c r="A10" s="17"/>
       <c r="B10"/>
       <c r="C10"/>
       <c r="D10"/>
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10"/>
-      <c r="H10" s="17"/>
-      <c r="L10" s="17"/>
-      <c r="O10" s="17"/>
-      <c r="P10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="18"/>
-      <c r="AC10" s="18"/>
-      <c r="AD10" s="18"/>
+      <c r="H10" s="43"/>
+      <c r="I10" s="41"/>
+      <c r="J10" s="41"/>
+      <c r="K10" s="41"/>
+      <c r="L10" s="43"/>
+      <c r="M10" s="41"/>
+      <c r="N10" s="41"/>
+      <c r="O10" s="43"/>
+      <c r="P10" s="44"/>
+      <c r="Q10" s="41"/>
+      <c r="R10" s="41"/>
+      <c r="S10" s="41"/>
+      <c r="T10" s="41"/>
+      <c r="U10" s="41"/>
+      <c r="V10" s="41"/>
+      <c r="W10" s="41"/>
+      <c r="X10" s="41"/>
+      <c r="Y10" s="41"/>
+      <c r="Z10" s="41"/>
+      <c r="AA10" s="44"/>
+      <c r="AB10" s="44"/>
+      <c r="AC10" s="44"/>
+      <c r="AD10" s="44"/>
     </row>
     <row r="11" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A11" s="20"/>
+      <c r="A11" s="17"/>
       <c r="B11"/>
       <c r="C11"/>
       <c r="D11"/>
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11"/>
-      <c r="H11" s="17"/>
-      <c r="L11" s="17"/>
-      <c r="O11" s="17"/>
-      <c r="P11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="18"/>
-      <c r="AC11" s="18"/>
-      <c r="AD11" s="18"/>
+      <c r="H11" s="43"/>
+      <c r="I11" s="41"/>
+      <c r="J11" s="41"/>
+      <c r="K11" s="41"/>
+      <c r="L11" s="43"/>
+      <c r="M11" s="41"/>
+      <c r="N11" s="41"/>
+      <c r="O11" s="43"/>
+      <c r="P11" s="44"/>
+      <c r="Q11" s="41"/>
+      <c r="R11" s="41"/>
+      <c r="S11" s="41"/>
+      <c r="T11" s="41"/>
+      <c r="U11" s="41"/>
+      <c r="V11" s="41"/>
+      <c r="W11" s="41"/>
+      <c r="X11" s="41"/>
+      <c r="Y11" s="41"/>
+      <c r="Z11" s="41"/>
+      <c r="AA11" s="44"/>
+      <c r="AB11" s="44"/>
+      <c r="AC11" s="44"/>
+      <c r="AD11" s="44"/>
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A12" s="20"/>
-      <c r="B12" s="39" t="s">
+      <c r="A12" s="17"/>
+      <c r="B12" s="34" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="39"/>
-      <c r="E12" s="39"/>
-      <c r="F12" s="39"/>
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="34"/>
+      <c r="F12" s="34"/>
       <c r="G12"/>
-      <c r="H12" s="17"/>
-      <c r="L12" s="17"/>
-      <c r="O12" s="17"/>
-      <c r="P12" s="18"/>
-      <c r="AA12" s="18"/>
-      <c r="AB12" s="18"/>
-      <c r="AC12" s="18"/>
-      <c r="AD12" s="18"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="41"/>
+      <c r="J12" s="41"/>
+      <c r="K12" s="41"/>
+      <c r="L12" s="43"/>
+      <c r="M12" s="41"/>
+      <c r="N12" s="41"/>
+      <c r="O12" s="43"/>
+      <c r="P12" s="44"/>
+      <c r="Q12" s="41"/>
+      <c r="R12" s="41"/>
+      <c r="S12" s="41"/>
+      <c r="T12" s="41"/>
+      <c r="U12" s="41"/>
+      <c r="V12" s="41"/>
+      <c r="W12" s="41"/>
+      <c r="X12" s="41"/>
+      <c r="Y12" s="41"/>
+      <c r="Z12" s="41"/>
+      <c r="AA12" s="44"/>
+      <c r="AB12" s="44"/>
+      <c r="AC12" s="44"/>
+      <c r="AD12" s="44"/>
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A13" s="20"/>
-      <c r="B13" s="38" t="s">
+      <c r="A13" s="17"/>
+      <c r="B13" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="34"/>
-      <c r="D13" s="34"/>
-      <c r="E13" s="34"/>
-      <c r="F13" s="34"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="32"/>
       <c r="G13"/>
-      <c r="H13" s="15"/>
-      <c r="L13" s="15"/>
-      <c r="O13" s="15"/>
-      <c r="P13" s="16"/>
-      <c r="AA13" s="16"/>
-      <c r="AB13" s="16"/>
-      <c r="AC13" s="16"/>
-      <c r="AD13" s="16"/>
+      <c r="H13" s="40"/>
+      <c r="I13" s="41"/>
+      <c r="J13" s="41"/>
+      <c r="K13" s="41"/>
+      <c r="L13" s="40"/>
+      <c r="M13" s="41"/>
+      <c r="N13" s="41"/>
+      <c r="O13" s="40"/>
+      <c r="P13" s="42"/>
+      <c r="Q13" s="41"/>
+      <c r="R13" s="41"/>
+      <c r="S13" s="41"/>
+      <c r="T13" s="41"/>
+      <c r="U13" s="41"/>
+      <c r="V13" s="41"/>
+      <c r="W13" s="41"/>
+      <c r="X13" s="41"/>
+      <c r="Y13" s="41"/>
+      <c r="Z13" s="41"/>
+      <c r="AA13" s="42"/>
+      <c r="AB13" s="42"/>
+      <c r="AC13" s="42"/>
+      <c r="AD13" s="42"/>
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A14" s="20"/>
-      <c r="B14" s="20"/>
-      <c r="C14" s="20"/>
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
       <c r="D14"/>
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14"/>
-      <c r="H14" s="17"/>
-      <c r="L14" s="17"/>
-      <c r="O14" s="17"/>
-      <c r="P14" s="18"/>
-      <c r="AA14" s="18"/>
-      <c r="AB14" s="18"/>
-      <c r="AC14" s="18"/>
-      <c r="AD14" s="18"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="41"/>
+      <c r="J14" s="41"/>
+      <c r="K14" s="41"/>
+      <c r="L14" s="43"/>
+      <c r="M14" s="41"/>
+      <c r="N14" s="41"/>
+      <c r="O14" s="43"/>
+      <c r="P14" s="44"/>
+      <c r="Q14" s="41"/>
+      <c r="R14" s="41"/>
+      <c r="S14" s="41"/>
+      <c r="T14" s="41"/>
+      <c r="U14" s="41"/>
+      <c r="V14" s="41"/>
+      <c r="W14" s="41"/>
+      <c r="X14" s="41"/>
+      <c r="Y14" s="41"/>
+      <c r="Z14" s="41"/>
+      <c r="AA14" s="44"/>
+      <c r="AB14" s="44"/>
+      <c r="AC14" s="44"/>
+      <c r="AD14" s="44"/>
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A15" s="20"/>
+      <c r="A15" s="17"/>
       <c r="B15"/>
       <c r="C15"/>
       <c r="D15"/>
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15"/>
-      <c r="H15" s="15"/>
-      <c r="L15" s="15"/>
-      <c r="O15" s="15"/>
-      <c r="P15" s="16"/>
-      <c r="AA15" s="16"/>
-      <c r="AB15" s="16"/>
-      <c r="AC15" s="16"/>
-      <c r="AD15" s="16"/>
+      <c r="H15" s="40"/>
+      <c r="I15" s="41"/>
+      <c r="J15" s="41"/>
+      <c r="K15" s="41"/>
+      <c r="L15" s="40"/>
+      <c r="M15" s="41"/>
+      <c r="N15" s="41"/>
+      <c r="O15" s="40"/>
+      <c r="P15" s="42"/>
+      <c r="Q15" s="41"/>
+      <c r="R15" s="41"/>
+      <c r="S15" s="41"/>
+      <c r="T15" s="41"/>
+      <c r="U15" s="41"/>
+      <c r="V15" s="41"/>
+      <c r="W15" s="41"/>
+      <c r="X15" s="41"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="42"/>
+      <c r="AB15" s="42"/>
+      <c r="AC15" s="42"/>
+      <c r="AD15" s="42"/>
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A16" s="20"/>
+      <c r="A16" s="17"/>
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="34"/>
-      <c r="F16" s="34"/>
+      <c r="C16" s="31"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="32"/>
       <c r="G16"/>
-      <c r="H16" s="15"/>
-      <c r="L16" s="15"/>
-      <c r="O16" s="15"/>
-      <c r="P16" s="16"/>
-      <c r="AA16" s="16"/>
-      <c r="AB16" s="16"/>
-      <c r="AC16" s="16"/>
-      <c r="AD16" s="16"/>
+      <c r="H16" s="40"/>
+      <c r="I16" s="41"/>
+      <c r="J16" s="41"/>
+      <c r="K16" s="41"/>
+      <c r="L16" s="40"/>
+      <c r="M16" s="41"/>
+      <c r="N16" s="41"/>
+      <c r="O16" s="40"/>
+      <c r="P16" s="42"/>
+      <c r="Q16" s="41"/>
+      <c r="R16" s="41"/>
+      <c r="S16" s="41"/>
+      <c r="T16" s="41"/>
+      <c r="U16" s="41"/>
+      <c r="V16" s="41"/>
+      <c r="W16" s="41"/>
+      <c r="X16" s="41"/>
+      <c r="Y16" s="41"/>
+      <c r="Z16" s="41"/>
+      <c r="AA16" s="42"/>
+      <c r="AB16" s="42"/>
+      <c r="AC16" s="42"/>
+      <c r="AD16" s="42"/>
     </row>
     <row r="17" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A17" s="20"/>
+      <c r="A17" s="17"/>
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="37"/>
-      <c r="D17" s="34"/>
-      <c r="E17" s="34"/>
-      <c r="F17" s="34"/>
+      <c r="C17" s="31"/>
+      <c r="D17" s="32"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="32"/>
       <c r="G17"/>
-      <c r="H17" s="19"/>
-      <c r="L17" s="15"/>
-      <c r="O17" s="15"/>
-      <c r="P17" s="16"/>
-      <c r="AA17" s="16"/>
-      <c r="AB17" s="16"/>
-      <c r="AC17" s="16"/>
-      <c r="AD17" s="16"/>
+      <c r="H17" s="45"/>
+      <c r="I17" s="41"/>
+      <c r="J17" s="41"/>
+      <c r="K17" s="41"/>
+      <c r="L17" s="40"/>
+      <c r="M17" s="41"/>
+      <c r="N17" s="41"/>
+      <c r="O17" s="40"/>
+      <c r="P17" s="42"/>
+      <c r="Q17" s="41"/>
+      <c r="R17" s="41"/>
+      <c r="S17" s="41"/>
+      <c r="T17" s="41"/>
+      <c r="U17" s="41"/>
+      <c r="V17" s="41"/>
+      <c r="W17" s="41"/>
+      <c r="X17" s="41"/>
+      <c r="Y17" s="41"/>
+      <c r="Z17" s="41"/>
+      <c r="AA17" s="42"/>
+      <c r="AB17" s="42"/>
+      <c r="AC17" s="42"/>
+      <c r="AD17" s="42"/>
     </row>
     <row r="18" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A18" s="20"/>
+      <c r="A18" s="17"/>
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="37"/>
-      <c r="D18" s="34"/>
-      <c r="E18" s="34"/>
-      <c r="F18" s="34"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="32"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="32"/>
       <c r="G18"/>
-      <c r="L18" s="15"/>
-      <c r="O18" s="15"/>
-      <c r="P18" s="16"/>
-      <c r="AA18" s="16"/>
-      <c r="AB18" s="16"/>
-      <c r="AC18" s="16"/>
-      <c r="AD18" s="16"/>
+      <c r="H18" s="41"/>
+      <c r="I18" s="41"/>
+      <c r="J18" s="41"/>
+      <c r="K18" s="41"/>
+      <c r="L18" s="40"/>
+      <c r="M18" s="41"/>
+      <c r="N18" s="41"/>
+      <c r="O18" s="40"/>
+      <c r="P18" s="42"/>
+      <c r="Q18" s="41"/>
+      <c r="R18" s="41"/>
+      <c r="S18" s="41"/>
+      <c r="T18" s="41"/>
+      <c r="U18" s="41"/>
+      <c r="V18" s="41"/>
+      <c r="W18" s="41"/>
+      <c r="X18" s="41"/>
+      <c r="Y18" s="41"/>
+      <c r="Z18" s="41"/>
+      <c r="AA18" s="42"/>
+      <c r="AB18" s="42"/>
+      <c r="AC18" s="42"/>
+      <c r="AD18" s="42"/>
     </row>
     <row r="19" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A19" s="20"/>
+      <c r="A19" s="17"/>
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="37"/>
-      <c r="D19" s="34"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
+      <c r="C19" s="31"/>
+      <c r="D19" s="32"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
       <c r="G19"/>
-      <c r="L19" s="15"/>
-      <c r="O19" s="15"/>
-      <c r="P19" s="16"/>
-      <c r="AA19" s="16"/>
-      <c r="AB19" s="16"/>
-      <c r="AC19" s="16"/>
-      <c r="AD19" s="16"/>
+      <c r="H19" s="41"/>
+      <c r="I19" s="41"/>
+      <c r="J19" s="41"/>
+      <c r="K19" s="41"/>
+      <c r="L19" s="40"/>
+      <c r="M19" s="41"/>
+      <c r="N19" s="41"/>
+      <c r="O19" s="40"/>
+      <c r="P19" s="42"/>
+      <c r="Q19" s="41"/>
+      <c r="R19" s="41"/>
+      <c r="S19" s="41"/>
+      <c r="T19" s="41"/>
+      <c r="U19" s="41"/>
+      <c r="V19" s="41"/>
+      <c r="W19" s="41"/>
+      <c r="X19" s="41"/>
+      <c r="Y19" s="41"/>
+      <c r="Z19" s="41"/>
+      <c r="AA19" s="42"/>
+      <c r="AB19" s="42"/>
+      <c r="AC19" s="42"/>
+      <c r="AD19" s="42"/>
     </row>
     <row r="20" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A20" s="20"/>
+      <c r="A20" s="17"/>
       <c r="B20"/>
       <c r="C20"/>
       <c r="D20"/>
       <c r="E20"/>
       <c r="F20"/>
       <c r="G20"/>
-      <c r="L20" s="15"/>
-      <c r="O20" s="15"/>
-      <c r="P20" s="16"/>
-      <c r="AA20" s="16"/>
-      <c r="AB20" s="16"/>
-      <c r="AC20" s="16"/>
-      <c r="AD20" s="16"/>
+      <c r="H20" s="41"/>
+      <c r="I20" s="41"/>
+      <c r="J20" s="41"/>
+      <c r="K20" s="41"/>
+      <c r="L20" s="40"/>
+      <c r="M20" s="41"/>
+      <c r="N20" s="41"/>
+      <c r="O20" s="40"/>
+      <c r="P20" s="42"/>
+      <c r="Q20" s="41"/>
+      <c r="R20" s="41"/>
+      <c r="S20" s="41"/>
+      <c r="T20" s="41"/>
+      <c r="U20" s="41"/>
+      <c r="V20" s="41"/>
+      <c r="W20" s="41"/>
+      <c r="X20" s="41"/>
+      <c r="Y20" s="41"/>
+      <c r="Z20" s="41"/>
+      <c r="AA20" s="42"/>
+      <c r="AB20" s="42"/>
+      <c r="AC20" s="42"/>
+      <c r="AD20" s="42"/>
     </row>
     <row r="21" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A21" s="20"/>
+      <c r="A21" s="17"/>
       <c r="B21"/>
       <c r="C21"/>
       <c r="D21"/>
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21"/>
-      <c r="H21" s="15"/>
-      <c r="L21" s="15"/>
-      <c r="O21" s="15"/>
-      <c r="P21" s="16"/>
-      <c r="AA21" s="16"/>
-      <c r="AB21" s="16"/>
-      <c r="AC21" s="16"/>
-      <c r="AD21" s="16"/>
+      <c r="H21" s="40"/>
+      <c r="I21" s="41"/>
+      <c r="J21" s="41"/>
+      <c r="K21" s="41"/>
+      <c r="L21" s="40"/>
+      <c r="M21" s="41"/>
+      <c r="N21" s="41"/>
+      <c r="O21" s="40"/>
+      <c r="P21" s="42"/>
+      <c r="Q21" s="41"/>
+      <c r="R21" s="41"/>
+      <c r="S21" s="41"/>
+      <c r="T21" s="41"/>
+      <c r="U21" s="41"/>
+      <c r="V21" s="41"/>
+      <c r="W21" s="41"/>
+      <c r="X21" s="41"/>
+      <c r="Y21" s="41"/>
+      <c r="Z21" s="41"/>
+      <c r="AA21" s="42"/>
+      <c r="AB21" s="42"/>
+      <c r="AC21" s="42"/>
+      <c r="AD21" s="42"/>
     </row>
     <row r="22" spans="1:30" ht="16" x14ac:dyDescent="0.2">
-      <c r="A22" s="20"/>
+      <c r="A22" s="17"/>
       <c r="B22" s="2" t="s">
         <v>19</v>
       </c>
@@ -1214,17 +1523,32 @@
       </c>
       <c r="F22"/>
       <c r="G22"/>
-      <c r="H22" s="15"/>
-      <c r="L22" s="15"/>
-      <c r="O22" s="15"/>
-      <c r="P22" s="16"/>
-      <c r="AA22" s="16"/>
-      <c r="AB22" s="16"/>
-      <c r="AC22" s="16"/>
-      <c r="AD22" s="16"/>
+      <c r="H22" s="40"/>
+      <c r="I22" s="41"/>
+      <c r="J22" s="41"/>
+      <c r="K22" s="41"/>
+      <c r="L22" s="40"/>
+      <c r="M22" s="41"/>
+      <c r="N22" s="41"/>
+      <c r="O22" s="40"/>
+      <c r="P22" s="42"/>
+      <c r="Q22" s="41"/>
+      <c r="R22" s="41"/>
+      <c r="S22" s="41"/>
+      <c r="T22" s="41"/>
+      <c r="U22" s="41"/>
+      <c r="V22" s="41"/>
+      <c r="W22" s="41"/>
+      <c r="X22" s="41"/>
+      <c r="Y22" s="41"/>
+      <c r="Z22" s="41"/>
+      <c r="AA22" s="42"/>
+      <c r="AB22" s="42"/>
+      <c r="AC22" s="42"/>
+      <c r="AD22" s="42"/>
     </row>
     <row r="23" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A23" s="20"/>
+      <c r="A23" s="17"/>
       <c r="B23" s="3" t="s">
         <v>21</v>
       </c>
@@ -1249,7 +1573,7 @@
       <c r="AD23" s="16"/>
     </row>
     <row r="24" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A24" s="20"/>
+      <c r="A24" s="17"/>
       <c r="B24" s="3" t="s">
         <v>22</v>
       </c>
@@ -1274,7 +1598,7 @@
       <c r="AD24" s="16"/>
     </row>
     <row r="25" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A25" s="20"/>
+      <c r="A25" s="17"/>
       <c r="B25" s="3" t="s">
         <v>23</v>
       </c>
@@ -1299,7 +1623,7 @@
       <c r="AD25" s="16"/>
     </row>
     <row r="26" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A26" s="20"/>
+      <c r="A26" s="17"/>
       <c r="B26" s="3" t="s">
         <v>28</v>
       </c>
@@ -1307,10 +1631,10 @@
         <v>0</v>
       </c>
       <c r="D26" s="13"/>
-      <c r="E26" s="40" t="s">
+      <c r="E26" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="41">
+      <c r="F26" s="30">
         <v>0</v>
       </c>
       <c r="G26"/>
@@ -1324,11 +1648,11 @@
       <c r="AD26" s="16"/>
     </row>
     <row r="27" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A27" s="20"/>
-      <c r="B27" s="29" t="s">
+      <c r="A27" s="17"/>
+      <c r="B27" s="25" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="30">
+      <c r="C27" s="26">
         <v>0</v>
       </c>
       <c r="D27"/>
@@ -1349,7 +1673,7 @@
       <c r="AD27" s="16"/>
     </row>
     <row r="28" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A28" s="20"/>
+      <c r="A28" s="17"/>
       <c r="B28" s="8" t="s">
         <v>25</v>
       </c>
@@ -1376,7 +1700,7 @@
       <c r="AD28" s="16"/>
     </row>
     <row r="29" spans="1:30" ht="13" x14ac:dyDescent="0.15">
-      <c r="A29" s="20"/>
+      <c r="A29" s="17"/>
       <c r="B29"/>
       <c r="C29"/>
       <c r="D29"/>
@@ -1393,7 +1717,7 @@
       <c r="AD29" s="16"/>
     </row>
     <row r="30" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
+      <c r="A30" s="17"/>
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
@@ -1415,7 +1739,7 @@
       <c r="AD30" s="16"/>
     </row>
     <row r="31" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A31" s="20"/>
+      <c r="A31" s="17"/>
       <c r="B31"/>
       <c r="C31"/>
       <c r="D31"/>
@@ -1432,10 +1756,10 @@
       <c r="AD31" s="16"/>
     </row>
     <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="28" t="s">
+      <c r="A32" s="24" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="27"/>
+      <c r="B32" s="23"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
@@ -5532,16 +5856,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="H1:K1"/>
+    <mergeCell ref="L1:O1"/>
+    <mergeCell ref="B1:F5"/>
+    <mergeCell ref="B9:F9"/>
+    <mergeCell ref="C17:F17"/>
     <mergeCell ref="C18:F18"/>
     <mergeCell ref="C19:F19"/>
     <mergeCell ref="B13:F13"/>
     <mergeCell ref="C16:F16"/>
     <mergeCell ref="B12:F12"/>
-    <mergeCell ref="H1:K1"/>
-    <mergeCell ref="L1:O1"/>
-    <mergeCell ref="B1:F5"/>
-    <mergeCell ref="B9:F9"/>
-    <mergeCell ref="C17:F17"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>

<commit_message>
Update Bon de commande
</commit_message>
<xml_diff>
--- a/assets/Bon_de_commande_THETYS.xlsx
+++ b/assets/Bon_de_commande_THETYS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/martinpuy/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{698926AD-7F7D-654E-B444-804D05539C0B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08FEC17D-4FE1-654C-A619-A5C8AFC7128C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1200" yWindow="460" windowWidth="27600" windowHeight="17540" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -322,14 +322,14 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
-        <bgColor rgb="FFCFE2F3"/>
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
+        <bgColor rgb="FFCFE2F3"/>
       </patternFill>
     </fill>
   </fills>
@@ -568,8 +568,6 @@
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -613,14 +611,8 @@
     <xf numFmtId="165" fontId="19" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="15" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -628,12 +620,20 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
@@ -944,7 +944,7 @@
   <dimension ref="A1:AE443"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="50" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -968,31 +968,31 @@
   <sheetData>
     <row r="1" spans="1:31" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="16"/>
-      <c r="B1" s="59"/>
-      <c r="C1" s="54"/>
-      <c r="D1" s="54"/>
-      <c r="E1" s="54"/>
-      <c r="F1" s="54"/>
+      <c r="B1" s="55"/>
+      <c r="C1" s="56"/>
+      <c r="D1" s="56"/>
+      <c r="E1" s="56"/>
+      <c r="F1" s="56"/>
       <c r="G1" s="16"/>
-      <c r="H1" s="57"/>
-      <c r="I1" s="58"/>
-      <c r="J1" s="58"/>
-      <c r="K1" s="58"/>
-      <c r="L1" s="57"/>
-      <c r="M1" s="58"/>
-      <c r="N1" s="58"/>
-      <c r="O1" s="58"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="54"/>
+      <c r="J1" s="54"/>
+      <c r="K1" s="54"/>
+      <c r="L1" s="53"/>
+      <c r="M1" s="54"/>
+      <c r="N1" s="54"/>
+      <c r="O1" s="54"/>
+      <c r="P1" s="37"/>
+      <c r="Q1" s="37"/>
+      <c r="R1" s="37"/>
     </row>
     <row r="2" spans="1:31" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="17"/>
-      <c r="B2" s="54"/>
-      <c r="C2" s="54"/>
-      <c r="D2" s="54"/>
-      <c r="E2" s="54"/>
-      <c r="F2" s="54"/>
+      <c r="B2" s="56"/>
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
       <c r="G2" s="16"/>
       <c r="H2" s="17"/>
       <c r="I2" s="17"/>
@@ -1002,13 +1002,13 @@
       <c r="M2" s="17"/>
       <c r="N2" s="17"/>
       <c r="O2" s="17"/>
-      <c r="P2" s="40" t="s">
+      <c r="P2" s="38" t="s">
         <v>0</v>
       </c>
-      <c r="Q2" s="41" t="s">
+      <c r="Q2" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="R2" s="40" t="s">
+      <c r="R2" s="38" t="s">
         <v>2</v>
       </c>
       <c r="S2" s="18" t="s">
@@ -1046,11 +1046,11 @@
     </row>
     <row r="3" spans="1:31" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="17"/>
-      <c r="B3" s="54"/>
-      <c r="C3" s="54"/>
-      <c r="D3" s="54"/>
-      <c r="E3" s="54"/>
-      <c r="F3" s="54"/>
+      <c r="B3" s="56"/>
+      <c r="C3" s="56"/>
+      <c r="D3" s="56"/>
+      <c r="E3" s="56"/>
+      <c r="F3" s="56"/>
       <c r="G3" s="16"/>
       <c r="H3" s="17"/>
       <c r="I3" s="17"/>
@@ -1060,15 +1060,15 @@
       <c r="M3" s="17"/>
       <c r="N3" s="17"/>
       <c r="O3" s="17"/>
-      <c r="P3" s="42">
+      <c r="P3" s="40">
         <f>R3+T3+G3</f>
         <v>0</v>
       </c>
-      <c r="Q3" s="43">
+      <c r="Q3" s="41">
         <f>SUM(H3:K3)</f>
         <v>0</v>
       </c>
-      <c r="R3" s="43">
+      <c r="R3" s="41">
         <f>24*2.5*X3+6*2.8333333333*Z3+Y3*3.2</f>
         <v>0</v>
       </c>
@@ -1118,11 +1118,11 @@
     </row>
     <row r="4" spans="1:31" s="18" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="16"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="54"/>
-      <c r="D4" s="54"/>
-      <c r="E4" s="54"/>
-      <c r="F4" s="54"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="56"/>
+      <c r="D4" s="56"/>
+      <c r="E4" s="56"/>
+      <c r="F4" s="56"/>
       <c r="G4" s="16"/>
       <c r="H4" s="17"/>
       <c r="I4" s="17"/>
@@ -1132,7 +1132,7 @@
       <c r="M4" s="17"/>
       <c r="N4" s="17"/>
       <c r="O4" s="17"/>
-      <c r="P4" s="33"/>
+      <c r="P4" s="31"/>
       <c r="Q4" s="17"/>
       <c r="R4" s="17"/>
       <c r="AA4" s="21"/>
@@ -1142,21 +1142,21 @@
     </row>
     <row r="5" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="16"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="54"/>
-      <c r="D5" s="54"/>
-      <c r="E5" s="54"/>
-      <c r="F5" s="54"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="56"/>
+      <c r="D5" s="56"/>
+      <c r="E5" s="56"/>
+      <c r="F5" s="56"/>
       <c r="G5" s="16"/>
-      <c r="H5" s="34"/>
+      <c r="H5" s="32"/>
       <c r="I5" s="16"/>
       <c r="J5" s="16"/>
       <c r="K5" s="16"/>
-      <c r="L5" s="34"/>
+      <c r="L5" s="32"/>
       <c r="M5" s="16"/>
       <c r="N5" s="16"/>
-      <c r="O5" s="34"/>
-      <c r="P5" s="35"/>
+      <c r="O5" s="32"/>
+      <c r="P5" s="33"/>
       <c r="Q5" s="16"/>
       <c r="R5" s="16"/>
       <c r="AA5" s="14"/>
@@ -1172,15 +1172,15 @@
       <c r="E6"/>
       <c r="F6"/>
       <c r="G6" s="16"/>
-      <c r="H6" s="34"/>
+      <c r="H6" s="32"/>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="16"/>
-      <c r="L6" s="34"/>
+      <c r="L6" s="32"/>
       <c r="M6" s="16"/>
       <c r="N6" s="16"/>
-      <c r="O6" s="34"/>
-      <c r="P6" s="35"/>
+      <c r="O6" s="32"/>
+      <c r="P6" s="33"/>
       <c r="Q6" s="16"/>
       <c r="R6" s="16"/>
       <c r="AA6" s="14"/>
@@ -1196,15 +1196,15 @@
       <c r="E7"/>
       <c r="F7"/>
       <c r="G7" s="16"/>
-      <c r="H7" s="34"/>
+      <c r="H7" s="32"/>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
       <c r="K7" s="16"/>
-      <c r="L7" s="34"/>
+      <c r="L7" s="32"/>
       <c r="M7" s="16"/>
       <c r="N7" s="16"/>
-      <c r="O7" s="34"/>
-      <c r="P7" s="35"/>
+      <c r="O7" s="32"/>
+      <c r="P7" s="33"/>
       <c r="Q7" s="16"/>
       <c r="R7" s="16"/>
       <c r="AA7" s="14"/>
@@ -1220,15 +1220,15 @@
       <c r="E8"/>
       <c r="F8"/>
       <c r="G8" s="16"/>
-      <c r="H8" s="34"/>
+      <c r="H8" s="32"/>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
       <c r="K8" s="16"/>
-      <c r="L8" s="34"/>
+      <c r="L8" s="32"/>
       <c r="M8" s="16"/>
       <c r="N8" s="16"/>
-      <c r="O8" s="34"/>
-      <c r="P8" s="35"/>
+      <c r="O8" s="32"/>
+      <c r="P8" s="33"/>
       <c r="Q8" s="16"/>
       <c r="R8" s="16"/>
       <c r="AA8" s="14"/>
@@ -1238,23 +1238,23 @@
     </row>
     <row r="9" spans="1:31" ht="20" x14ac:dyDescent="0.2">
       <c r="A9" s="16"/>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="57" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="61"/>
-      <c r="E9" s="61"/>
-      <c r="F9" s="61"/>
+      <c r="C9" s="58"/>
+      <c r="D9" s="58"/>
+      <c r="E9" s="58"/>
+      <c r="F9" s="58"/>
       <c r="G9" s="16"/>
-      <c r="H9" s="34"/>
+      <c r="H9" s="32"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
       <c r="K9" s="16"/>
-      <c r="L9" s="34"/>
+      <c r="L9" s="32"/>
       <c r="M9" s="16"/>
       <c r="N9" s="16"/>
-      <c r="O9" s="34"/>
-      <c r="P9" s="35"/>
+      <c r="O9" s="32"/>
+      <c r="P9" s="33"/>
       <c r="Q9" s="16"/>
       <c r="R9" s="16"/>
       <c r="AA9" s="14"/>
@@ -1270,15 +1270,15 @@
       <c r="E10"/>
       <c r="F10"/>
       <c r="G10" s="16"/>
-      <c r="H10" s="36"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="16"/>
       <c r="J10" s="16"/>
       <c r="K10" s="16"/>
-      <c r="L10" s="36"/>
+      <c r="L10" s="34"/>
       <c r="M10" s="16"/>
       <c r="N10" s="16"/>
-      <c r="O10" s="36"/>
-      <c r="P10" s="37"/>
+      <c r="O10" s="34"/>
+      <c r="P10" s="35"/>
       <c r="Q10" s="16"/>
       <c r="R10" s="16"/>
       <c r="AA10" s="15"/>
@@ -1294,15 +1294,15 @@
       <c r="E11"/>
       <c r="F11"/>
       <c r="G11" s="16"/>
-      <c r="H11" s="36"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="16"/>
       <c r="J11" s="16"/>
       <c r="K11" s="16"/>
-      <c r="L11" s="36"/>
+      <c r="L11" s="34"/>
       <c r="M11" s="16"/>
       <c r="N11" s="16"/>
-      <c r="O11" s="36"/>
-      <c r="P11" s="37"/>
+      <c r="O11" s="34"/>
+      <c r="P11" s="35"/>
       <c r="Q11" s="16"/>
       <c r="R11" s="16"/>
       <c r="AA11" s="15"/>
@@ -1312,23 +1312,23 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A12" s="16"/>
-      <c r="B12" s="56" t="s">
+      <c r="B12" s="61" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="56"/>
-      <c r="D12" s="56"/>
-      <c r="E12" s="56"/>
-      <c r="F12" s="56"/>
+      <c r="C12" s="61"/>
+      <c r="D12" s="61"/>
+      <c r="E12" s="61"/>
+      <c r="F12" s="61"/>
       <c r="G12" s="16"/>
-      <c r="H12" s="36"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="16"/>
       <c r="J12" s="16"/>
       <c r="K12" s="16"/>
-      <c r="L12" s="36"/>
+      <c r="L12" s="34"/>
       <c r="M12" s="16"/>
       <c r="N12" s="16"/>
-      <c r="O12" s="36"/>
-      <c r="P12" s="37"/>
+      <c r="O12" s="34"/>
+      <c r="P12" s="35"/>
       <c r="Q12" s="16"/>
       <c r="R12" s="16"/>
       <c r="AA12" s="15"/>
@@ -1338,23 +1338,23 @@
     </row>
     <row r="13" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A13" s="16"/>
-      <c r="B13" s="55" t="s">
+      <c r="B13" s="60" t="s">
         <v>30</v>
       </c>
-      <c r="C13" s="54"/>
-      <c r="D13" s="54"/>
-      <c r="E13" s="54"/>
-      <c r="F13" s="54"/>
+      <c r="C13" s="56"/>
+      <c r="D13" s="56"/>
+      <c r="E13" s="56"/>
+      <c r="F13" s="56"/>
       <c r="G13" s="16"/>
-      <c r="H13" s="34"/>
+      <c r="H13" s="32"/>
       <c r="I13" s="16"/>
       <c r="J13" s="16"/>
       <c r="K13" s="16"/>
-      <c r="L13" s="34"/>
+      <c r="L13" s="32"/>
       <c r="M13" s="16"/>
       <c r="N13" s="16"/>
-      <c r="O13" s="34"/>
-      <c r="P13" s="35"/>
+      <c r="O13" s="32"/>
+      <c r="P13" s="33"/>
       <c r="Q13" s="16"/>
       <c r="R13" s="16"/>
       <c r="AA13" s="14"/>
@@ -1370,15 +1370,15 @@
       <c r="E14"/>
       <c r="F14"/>
       <c r="G14" s="16"/>
-      <c r="H14" s="36"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="16"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
-      <c r="L14" s="36"/>
+      <c r="L14" s="34"/>
       <c r="M14" s="16"/>
       <c r="N14" s="16"/>
-      <c r="O14" s="36"/>
-      <c r="P14" s="37"/>
+      <c r="O14" s="34"/>
+      <c r="P14" s="35"/>
       <c r="Q14" s="16"/>
       <c r="R14" s="16"/>
       <c r="AA14" s="15"/>
@@ -1394,15 +1394,15 @@
       <c r="E15"/>
       <c r="F15"/>
       <c r="G15" s="16"/>
-      <c r="H15" s="34"/>
+      <c r="H15" s="32"/>
       <c r="I15" s="16"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
-      <c r="L15" s="34"/>
+      <c r="L15" s="32"/>
       <c r="M15" s="16"/>
       <c r="N15" s="16"/>
-      <c r="O15" s="34"/>
-      <c r="P15" s="35"/>
+      <c r="O15" s="32"/>
+      <c r="P15" s="33"/>
       <c r="Q15" s="16"/>
       <c r="R15" s="16"/>
       <c r="AA15" s="14"/>
@@ -1415,20 +1415,20 @@
       <c r="B16" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C16" s="53"/>
-      <c r="D16" s="54"/>
-      <c r="E16" s="54"/>
-      <c r="F16" s="54"/>
+      <c r="C16" s="59"/>
+      <c r="D16" s="56"/>
+      <c r="E16" s="56"/>
+      <c r="F16" s="56"/>
       <c r="G16" s="16"/>
-      <c r="H16" s="34"/>
+      <c r="H16" s="32"/>
       <c r="I16" s="16"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
-      <c r="L16" s="34"/>
+      <c r="L16" s="32"/>
       <c r="M16" s="16"/>
       <c r="N16" s="16"/>
-      <c r="O16" s="34"/>
-      <c r="P16" s="35"/>
+      <c r="O16" s="32"/>
+      <c r="P16" s="33"/>
       <c r="Q16" s="16"/>
       <c r="R16" s="16"/>
       <c r="AA16" s="14"/>
@@ -1441,20 +1441,20 @@
       <c r="B17" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C17" s="53"/>
-      <c r="D17" s="54"/>
-      <c r="E17" s="54"/>
-      <c r="F17" s="54"/>
+      <c r="C17" s="59"/>
+      <c r="D17" s="56"/>
+      <c r="E17" s="56"/>
+      <c r="F17" s="56"/>
       <c r="G17" s="16"/>
-      <c r="H17" s="38"/>
+      <c r="H17" s="36"/>
       <c r="I17" s="16"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" s="34"/>
+      <c r="L17" s="32"/>
       <c r="M17" s="16"/>
       <c r="N17" s="16"/>
-      <c r="O17" s="34"/>
-      <c r="P17" s="35"/>
+      <c r="O17" s="32"/>
+      <c r="P17" s="33"/>
       <c r="Q17" s="16"/>
       <c r="R17" s="16"/>
       <c r="AA17" s="14"/>
@@ -1467,20 +1467,20 @@
       <c r="B18" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="53"/>
-      <c r="D18" s="54"/>
-      <c r="E18" s="54"/>
-      <c r="F18" s="54"/>
+      <c r="C18" s="59"/>
+      <c r="D18" s="56"/>
+      <c r="E18" s="56"/>
+      <c r="F18" s="56"/>
       <c r="G18" s="16"/>
       <c r="H18" s="16"/>
       <c r="I18" s="16"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" s="34"/>
+      <c r="L18" s="32"/>
       <c r="M18" s="16"/>
       <c r="N18" s="16"/>
-      <c r="O18" s="34"/>
-      <c r="P18" s="35"/>
+      <c r="O18" s="32"/>
+      <c r="P18" s="33"/>
       <c r="Q18" s="16"/>
       <c r="R18" s="16"/>
       <c r="AA18" s="14"/>
@@ -1493,20 +1493,20 @@
       <c r="B19" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="53"/>
-      <c r="D19" s="54"/>
-      <c r="E19" s="54"/>
-      <c r="F19" s="54"/>
+      <c r="C19" s="59"/>
+      <c r="D19" s="56"/>
+      <c r="E19" s="56"/>
+      <c r="F19" s="56"/>
       <c r="G19" s="16"/>
       <c r="H19" s="16"/>
       <c r="I19" s="16"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" s="34"/>
+      <c r="L19" s="32"/>
       <c r="M19" s="16"/>
       <c r="N19" s="16"/>
-      <c r="O19" s="34"/>
-      <c r="P19" s="35"/>
+      <c r="O19" s="32"/>
+      <c r="P19" s="33"/>
       <c r="Q19" s="16"/>
       <c r="R19" s="16"/>
       <c r="AA19" s="14"/>
@@ -1526,11 +1526,11 @@
       <c r="I20" s="16"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
-      <c r="L20" s="34"/>
+      <c r="L20" s="32"/>
       <c r="M20" s="16"/>
       <c r="N20" s="16"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="35"/>
+      <c r="O20" s="32"/>
+      <c r="P20" s="33"/>
       <c r="Q20" s="16"/>
       <c r="R20" s="16"/>
       <c r="AA20" s="14"/>
@@ -1546,15 +1546,15 @@
       <c r="E21"/>
       <c r="F21"/>
       <c r="G21" s="16"/>
-      <c r="H21" s="34"/>
+      <c r="H21" s="32"/>
       <c r="I21" s="16"/>
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
-      <c r="L21" s="34"/>
+      <c r="L21" s="32"/>
       <c r="M21" s="16"/>
       <c r="N21" s="16"/>
-      <c r="O21" s="34"/>
-      <c r="P21" s="35"/>
+      <c r="O21" s="32"/>
+      <c r="P21" s="33"/>
       <c r="Q21" s="16"/>
       <c r="R21" s="16"/>
       <c r="AA21" s="14"/>
@@ -1574,15 +1574,15 @@
       </c>
       <c r="F22"/>
       <c r="G22" s="16"/>
-      <c r="H22" s="34"/>
+      <c r="H22" s="32"/>
       <c r="I22" s="16"/>
       <c r="J22" s="16"/>
       <c r="K22" s="16"/>
-      <c r="L22" s="34"/>
+      <c r="L22" s="32"/>
       <c r="M22" s="16"/>
       <c r="N22" s="16"/>
-      <c r="O22" s="34"/>
-      <c r="P22" s="35"/>
+      <c r="O22" s="32"/>
+      <c r="P22" s="33"/>
       <c r="Q22" s="16"/>
       <c r="R22" s="16"/>
       <c r="AA22" s="14"/>
@@ -1606,15 +1606,15 @@
         <v>0</v>
       </c>
       <c r="G23" s="16"/>
-      <c r="H23" s="34"/>
+      <c r="H23" s="32"/>
       <c r="I23" s="16"/>
       <c r="J23" s="16"/>
       <c r="K23" s="16"/>
-      <c r="L23" s="34"/>
+      <c r="L23" s="32"/>
       <c r="M23" s="16"/>
       <c r="N23" s="16"/>
-      <c r="O23" s="34"/>
-      <c r="P23" s="35"/>
+      <c r="O23" s="32"/>
+      <c r="P23" s="33"/>
       <c r="Q23" s="16"/>
       <c r="R23" s="16"/>
       <c r="AA23" s="14"/>
@@ -1638,15 +1638,15 @@
         <v>0</v>
       </c>
       <c r="G24" s="16"/>
-      <c r="H24" s="34"/>
+      <c r="H24" s="32"/>
       <c r="I24" s="16"/>
       <c r="J24" s="16"/>
       <c r="K24" s="16"/>
-      <c r="L24" s="34"/>
+      <c r="L24" s="32"/>
       <c r="M24" s="16"/>
       <c r="N24" s="16"/>
-      <c r="O24" s="34"/>
-      <c r="P24" s="35"/>
+      <c r="O24" s="32"/>
+      <c r="P24" s="33"/>
       <c r="Q24" s="16"/>
       <c r="R24" s="16"/>
       <c r="AA24" s="14"/>
@@ -1670,15 +1670,15 @@
         <v>0</v>
       </c>
       <c r="G25" s="16"/>
-      <c r="H25" s="34"/>
+      <c r="H25" s="32"/>
       <c r="I25" s="16"/>
       <c r="J25" s="16"/>
       <c r="K25" s="16"/>
-      <c r="L25" s="34"/>
+      <c r="L25" s="32"/>
       <c r="M25" s="16"/>
       <c r="N25" s="16"/>
-      <c r="O25" s="34"/>
-      <c r="P25" s="35"/>
+      <c r="O25" s="32"/>
+      <c r="P25" s="33"/>
       <c r="Q25" s="16"/>
       <c r="R25" s="16"/>
       <c r="AA25" s="14"/>
@@ -1688,29 +1688,29 @@
     </row>
     <row r="26" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A26" s="16"/>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="62" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="23">
+      <c r="C26" s="64">
         <v>0</v>
       </c>
       <c r="D26" s="11"/>
-      <c r="E26" s="62" t="s">
+      <c r="E26" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="F26" s="23">
+      <c r="F26" s="64">
         <v>0</v>
       </c>
       <c r="G26" s="16"/>
-      <c r="H26" s="34"/>
+      <c r="H26" s="32"/>
       <c r="I26" s="16"/>
       <c r="J26" s="16"/>
       <c r="K26" s="16"/>
-      <c r="L26" s="34"/>
+      <c r="L26" s="32"/>
       <c r="M26" s="16"/>
       <c r="N26" s="16"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="35"/>
+      <c r="O26" s="32"/>
+      <c r="P26" s="33"/>
       <c r="Q26" s="16"/>
       <c r="R26" s="16"/>
       <c r="AA26" s="14"/>
@@ -1720,29 +1720,29 @@
     </row>
     <row r="27" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A27" s="16"/>
-      <c r="B27" s="63" t="s">
+      <c r="B27" s="51" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="64">
+      <c r="C27" s="52">
         <v>0</v>
       </c>
       <c r="D27"/>
-      <c r="E27" s="62" t="s">
+      <c r="E27" s="63" t="s">
         <v>24</v>
       </c>
-      <c r="F27" s="23">
+      <c r="F27" s="64">
         <v>0</v>
       </c>
       <c r="G27" s="16"/>
-      <c r="H27" s="34"/>
+      <c r="H27" s="32"/>
       <c r="I27" s="16"/>
       <c r="J27" s="16"/>
       <c r="K27" s="16"/>
-      <c r="L27" s="34"/>
+      <c r="L27" s="32"/>
       <c r="M27" s="16"/>
       <c r="N27" s="16"/>
-      <c r="O27" s="34"/>
-      <c r="P27" s="35"/>
+      <c r="O27" s="32"/>
+      <c r="P27" s="33"/>
       <c r="Q27" s="16"/>
       <c r="R27" s="16"/>
       <c r="AA27" s="14"/>
@@ -1768,15 +1768,15 @@
         <v>0</v>
       </c>
       <c r="G28" s="16"/>
-      <c r="H28" s="34"/>
+      <c r="H28" s="32"/>
       <c r="I28" s="16"/>
       <c r="J28" s="16"/>
       <c r="K28" s="16"/>
-      <c r="L28" s="34"/>
+      <c r="L28" s="32"/>
       <c r="M28" s="16"/>
       <c r="N28" s="16"/>
-      <c r="O28" s="34"/>
-      <c r="P28" s="35"/>
+      <c r="O28" s="32"/>
+      <c r="P28" s="33"/>
       <c r="Q28" s="16"/>
       <c r="R28" s="16"/>
       <c r="AA28" s="14"/>
@@ -1792,15 +1792,15 @@
       <c r="E29"/>
       <c r="F29"/>
       <c r="G29" s="16"/>
-      <c r="H29" s="34"/>
+      <c r="H29" s="32"/>
       <c r="I29" s="16"/>
       <c r="J29" s="16"/>
       <c r="K29" s="16"/>
-      <c r="L29" s="34"/>
+      <c r="L29" s="32"/>
       <c r="M29" s="16"/>
       <c r="N29" s="16"/>
-      <c r="O29" s="34"/>
-      <c r="P29" s="35"/>
+      <c r="O29" s="32"/>
+      <c r="P29" s="33"/>
       <c r="Q29" s="16"/>
       <c r="R29" s="16"/>
       <c r="AA29" s="14"/>
@@ -1813,23 +1813,23 @@
       <c r="B30"/>
       <c r="C30"/>
       <c r="D30"/>
-      <c r="E30" s="44" t="s">
+      <c r="E30" s="42" t="s">
         <v>27</v>
       </c>
-      <c r="F30" s="45">
+      <c r="F30" s="43">
         <f>P3</f>
         <v>0</v>
       </c>
       <c r="G30" s="16"/>
-      <c r="H30" s="34"/>
+      <c r="H30" s="32"/>
       <c r="I30" s="16"/>
       <c r="J30" s="16"/>
       <c r="K30" s="16"/>
-      <c r="L30" s="34"/>
+      <c r="L30" s="32"/>
       <c r="M30" s="16"/>
       <c r="N30" s="16"/>
-      <c r="O30" s="34"/>
-      <c r="P30" s="35"/>
+      <c r="O30" s="32"/>
+      <c r="P30" s="33"/>
       <c r="Q30" s="16"/>
       <c r="R30" s="16"/>
       <c r="AA30" s="14"/>
@@ -1845,15 +1845,15 @@
       <c r="E31"/>
       <c r="F31"/>
       <c r="G31" s="16"/>
-      <c r="H31" s="34"/>
+      <c r="H31" s="32"/>
       <c r="I31" s="16"/>
       <c r="J31" s="16"/>
       <c r="K31" s="16"/>
-      <c r="L31" s="34"/>
+      <c r="L31" s="32"/>
       <c r="M31" s="16"/>
       <c r="N31" s="16"/>
-      <c r="O31" s="34"/>
-      <c r="P31" s="35"/>
+      <c r="O31" s="32"/>
+      <c r="P31" s="33"/>
       <c r="Q31" s="16"/>
       <c r="R31" s="16"/>
       <c r="AA31" s="14"/>
@@ -1862,24 +1862,24 @@
       <c r="AD31" s="14"/>
     </row>
     <row r="32" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A32" s="25" t="s">
+      <c r="A32" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="B32" s="24"/>
+      <c r="B32" s="22"/>
       <c r="C32"/>
       <c r="D32"/>
       <c r="E32"/>
       <c r="F32"/>
       <c r="G32" s="16"/>
-      <c r="H32" s="34"/>
+      <c r="H32" s="32"/>
       <c r="I32" s="16"/>
       <c r="J32" s="16"/>
       <c r="K32" s="16"/>
-      <c r="L32" s="34"/>
+      <c r="L32" s="32"/>
       <c r="M32" s="16"/>
       <c r="N32" s="16"/>
-      <c r="O32" s="34"/>
-      <c r="P32" s="35"/>
+      <c r="O32" s="32"/>
+      <c r="P32" s="33"/>
       <c r="Q32" s="16"/>
       <c r="R32" s="16"/>
       <c r="AA32" s="14"/>
@@ -1890,20 +1890,20 @@
     <row r="33" spans="1:30" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A33" s="16"/>
       <c r="B33" s="16"/>
-      <c r="C33" s="26"/>
-      <c r="D33" s="26"/>
-      <c r="E33" s="26"/>
-      <c r="F33" s="26"/>
+      <c r="C33" s="24"/>
+      <c r="D33" s="24"/>
+      <c r="E33" s="24"/>
+      <c r="F33" s="24"/>
       <c r="G33" s="16"/>
-      <c r="H33" s="34"/>
+      <c r="H33" s="32"/>
       <c r="I33" s="16"/>
       <c r="J33" s="16"/>
       <c r="K33" s="16"/>
-      <c r="L33" s="34"/>
+      <c r="L33" s="32"/>
       <c r="M33" s="16"/>
       <c r="N33" s="16"/>
-      <c r="O33" s="34"/>
-      <c r="P33" s="35"/>
+      <c r="O33" s="32"/>
+      <c r="P33" s="33"/>
       <c r="Q33" s="16"/>
       <c r="R33" s="16"/>
       <c r="AA33" s="14"/>
@@ -1914,20 +1914,20 @@
     <row r="34" spans="1:30" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A34" s="16"/>
       <c r="B34" s="16"/>
-      <c r="C34" s="26"/>
-      <c r="D34" s="26"/>
-      <c r="E34" s="26"/>
-      <c r="F34" s="26"/>
+      <c r="C34" s="24"/>
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="24"/>
       <c r="G34" s="16"/>
-      <c r="H34" s="34"/>
+      <c r="H34" s="32"/>
       <c r="I34" s="16"/>
       <c r="J34" s="16"/>
       <c r="K34" s="16"/>
-      <c r="L34" s="34"/>
+      <c r="L34" s="32"/>
       <c r="M34" s="16"/>
       <c r="N34" s="16"/>
-      <c r="O34" s="34"/>
-      <c r="P34" s="35"/>
+      <c r="O34" s="32"/>
+      <c r="P34" s="33"/>
       <c r="Q34" s="16"/>
       <c r="R34" s="16"/>
       <c r="AA34" s="14"/>
@@ -1937,21 +1937,21 @@
     </row>
     <row r="35" spans="1:30" ht="11" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A35" s="16"/>
-      <c r="B35" s="31"/>
-      <c r="C35" s="31"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="31"/>
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="29"/>
+      <c r="E35" s="29"/>
+      <c r="F35" s="29"/>
       <c r="G35" s="16"/>
-      <c r="H35" s="34"/>
+      <c r="H35" s="32"/>
       <c r="I35" s="16"/>
       <c r="J35" s="16"/>
       <c r="K35" s="16"/>
-      <c r="L35" s="34"/>
+      <c r="L35" s="32"/>
       <c r="M35" s="16"/>
       <c r="N35" s="16"/>
-      <c r="O35" s="34"/>
-      <c r="P35" s="35"/>
+      <c r="O35" s="32"/>
+      <c r="P35" s="33"/>
       <c r="Q35" s="16"/>
       <c r="R35" s="16"/>
       <c r="AA35" s="14"/>
@@ -1963,21 +1963,21 @@
       <c r="A36" s="16"/>
       <c r="B36" s="16"/>
       <c r="C36" s="16"/>
-      <c r="D36" s="30" t="s">
+      <c r="D36" s="28" t="s">
         <v>31</v>
       </c>
       <c r="E36" s="16"/>
       <c r="F36" s="16"/>
       <c r="G36" s="16"/>
-      <c r="H36" s="34"/>
+      <c r="H36" s="32"/>
       <c r="I36" s="16"/>
       <c r="J36" s="16"/>
       <c r="K36" s="16"/>
-      <c r="L36" s="34"/>
+      <c r="L36" s="32"/>
       <c r="M36" s="16"/>
       <c r="N36" s="16"/>
-      <c r="O36" s="34"/>
-      <c r="P36" s="35"/>
+      <c r="O36" s="32"/>
+      <c r="P36" s="33"/>
       <c r="Q36" s="16"/>
       <c r="R36" s="16"/>
       <c r="AA36" s="14"/>
@@ -1993,15 +1993,15 @@
       <c r="E37" s="16"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
-      <c r="H37" s="34"/>
+      <c r="H37" s="32"/>
       <c r="I37" s="16"/>
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
-      <c r="L37" s="34"/>
+      <c r="L37" s="32"/>
       <c r="M37" s="16"/>
       <c r="N37" s="16"/>
-      <c r="O37" s="34"/>
-      <c r="P37" s="35"/>
+      <c r="O37" s="32"/>
+      <c r="P37" s="33"/>
       <c r="Q37" s="16"/>
       <c r="R37" s="16"/>
       <c r="AA37" s="14"/>
@@ -2012,24 +2012,24 @@
     <row r="38" spans="1:30" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="16"/>
       <c r="B38" s="16"/>
-      <c r="C38" s="49" t="s">
+      <c r="C38" s="47" t="s">
         <v>19</v>
       </c>
       <c r="D38" s="16"/>
       <c r="E38" s="16"/>
-      <c r="F38" s="49" t="s">
+      <c r="F38" s="47" t="s">
         <v>20</v>
       </c>
       <c r="G38" s="16"/>
-      <c r="H38" s="34"/>
+      <c r="H38" s="32"/>
       <c r="I38" s="16"/>
       <c r="J38" s="16"/>
       <c r="K38" s="16"/>
-      <c r="L38" s="34"/>
+      <c r="L38" s="32"/>
       <c r="M38" s="16"/>
       <c r="N38" s="16"/>
-      <c r="O38" s="34"/>
-      <c r="P38" s="35"/>
+      <c r="O38" s="32"/>
+      <c r="P38" s="33"/>
       <c r="Q38" s="16"/>
       <c r="R38" s="16"/>
       <c r="AA38" s="14"/>
@@ -2039,29 +2039,29 @@
     </row>
     <row r="39" spans="1:30" ht="23" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A39" s="16"/>
-      <c r="B39" s="27" t="s">
+      <c r="B39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="C39" s="46">
+      <c r="C39" s="44">
         <v>3.2</v>
       </c>
       <c r="D39" s="16"/>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="25" t="s">
         <v>32</v>
       </c>
-      <c r="F39" s="46">
+      <c r="F39" s="44">
         <v>6.8</v>
       </c>
       <c r="G39" s="16"/>
-      <c r="H39" s="34"/>
+      <c r="H39" s="32"/>
       <c r="I39" s="16"/>
       <c r="J39" s="16"/>
       <c r="K39" s="16"/>
-      <c r="L39" s="34"/>
+      <c r="L39" s="32"/>
       <c r="M39" s="16"/>
       <c r="N39" s="16"/>
-      <c r="O39" s="34"/>
-      <c r="P39" s="35"/>
+      <c r="O39" s="32"/>
+      <c r="P39" s="33"/>
       <c r="Q39" s="16"/>
       <c r="R39" s="16"/>
       <c r="AA39" s="14"/>
@@ -2071,29 +2071,29 @@
     </row>
     <row r="40" spans="1:30" ht="20" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A40" s="16"/>
-      <c r="B40" s="28" t="s">
+      <c r="B40" s="26" t="s">
         <v>33</v>
       </c>
-      <c r="C40" s="47">
+      <c r="C40" s="45">
         <v>17</v>
       </c>
       <c r="D40" s="16"/>
-      <c r="E40" s="50" t="s">
+      <c r="E40" s="48" t="s">
         <v>35</v>
       </c>
-      <c r="F40" s="52">
+      <c r="F40" s="50">
         <v>17.5</v>
       </c>
       <c r="G40" s="16"/>
-      <c r="H40" s="34"/>
+      <c r="H40" s="32"/>
       <c r="I40" s="16"/>
       <c r="J40" s="16"/>
       <c r="K40" s="16"/>
-      <c r="L40" s="34"/>
+      <c r="L40" s="32"/>
       <c r="M40" s="16"/>
       <c r="N40" s="16"/>
-      <c r="O40" s="34"/>
-      <c r="P40" s="35"/>
+      <c r="O40" s="32"/>
+      <c r="P40" s="33"/>
       <c r="Q40" s="16"/>
       <c r="R40" s="16"/>
       <c r="AA40" s="14"/>
@@ -2103,29 +2103,29 @@
     </row>
     <row r="41" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A41" s="16"/>
-      <c r="B41" s="29" t="s">
+      <c r="B41" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="C41" s="48">
+      <c r="C41" s="46">
         <v>60</v>
       </c>
       <c r="D41" s="16"/>
-      <c r="E41" s="51" t="s">
+      <c r="E41" s="49" t="s">
         <v>33</v>
       </c>
-      <c r="F41" s="48">
+      <c r="F41" s="46">
         <v>30</v>
       </c>
       <c r="G41" s="16"/>
-      <c r="H41" s="34"/>
+      <c r="H41" s="32"/>
       <c r="I41" s="16"/>
       <c r="J41" s="16"/>
       <c r="K41" s="16"/>
-      <c r="L41" s="34"/>
+      <c r="L41" s="32"/>
       <c r="M41" s="16"/>
       <c r="N41" s="16"/>
-      <c r="O41" s="34"/>
-      <c r="P41" s="35"/>
+      <c r="O41" s="32"/>
+      <c r="P41" s="33"/>
       <c r="Q41" s="16"/>
       <c r="R41" s="16"/>
       <c r="AA41" s="14"/>
@@ -2141,15 +2141,15 @@
       <c r="E42" s="16"/>
       <c r="F42" s="16"/>
       <c r="G42" s="16"/>
-      <c r="H42" s="34"/>
+      <c r="H42" s="32"/>
       <c r="I42" s="16"/>
       <c r="J42" s="16"/>
       <c r="K42" s="16"/>
-      <c r="L42" s="34"/>
+      <c r="L42" s="32"/>
       <c r="M42" s="16"/>
       <c r="N42" s="16"/>
-      <c r="O42" s="34"/>
-      <c r="P42" s="35"/>
+      <c r="O42" s="32"/>
+      <c r="P42" s="33"/>
       <c r="Q42" s="16"/>
       <c r="R42" s="16"/>
       <c r="AA42" s="14"/>
@@ -2165,15 +2165,15 @@
       <c r="E43" s="16"/>
       <c r="F43" s="16"/>
       <c r="G43" s="16"/>
-      <c r="H43" s="34"/>
+      <c r="H43" s="32"/>
       <c r="I43" s="16"/>
       <c r="J43" s="16"/>
       <c r="K43" s="16"/>
-      <c r="L43" s="34"/>
+      <c r="L43" s="32"/>
       <c r="M43" s="16"/>
       <c r="N43" s="16"/>
-      <c r="O43" s="34"/>
-      <c r="P43" s="35"/>
+      <c r="O43" s="32"/>
+      <c r="P43" s="33"/>
       <c r="Q43" s="16"/>
       <c r="R43" s="16"/>
       <c r="AA43" s="14"/>
@@ -2189,15 +2189,15 @@
       <c r="E44" s="16"/>
       <c r="F44" s="16"/>
       <c r="G44" s="16"/>
-      <c r="H44" s="34"/>
+      <c r="H44" s="32"/>
       <c r="I44" s="16"/>
       <c r="J44" s="16"/>
       <c r="K44" s="16"/>
-      <c r="L44" s="34"/>
+      <c r="L44" s="32"/>
       <c r="M44" s="16"/>
       <c r="N44" s="16"/>
-      <c r="O44" s="34"/>
-      <c r="P44" s="35"/>
+      <c r="O44" s="32"/>
+      <c r="P44" s="33"/>
       <c r="Q44" s="16"/>
       <c r="R44" s="16"/>
       <c r="AA44" s="14"/>
@@ -2213,15 +2213,15 @@
       <c r="E45" s="16"/>
       <c r="F45" s="16"/>
       <c r="G45" s="16"/>
-      <c r="H45" s="34"/>
+      <c r="H45" s="32"/>
       <c r="I45" s="16"/>
       <c r="J45" s="16"/>
       <c r="K45" s="16"/>
-      <c r="L45" s="34"/>
+      <c r="L45" s="32"/>
       <c r="M45" s="16"/>
       <c r="N45" s="16"/>
-      <c r="O45" s="34"/>
-      <c r="P45" s="35"/>
+      <c r="O45" s="32"/>
+      <c r="P45" s="33"/>
       <c r="Q45" s="16"/>
       <c r="R45" s="16"/>
       <c r="AA45" s="14"/>
@@ -2230,13 +2230,13 @@
       <c r="AD45" s="14"/>
     </row>
     <row r="46" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A46" s="32"/>
-      <c r="B46" s="32"/>
-      <c r="C46" s="32"/>
-      <c r="D46" s="32"/>
-      <c r="E46" s="32"/>
-      <c r="F46" s="32"/>
-      <c r="G46" s="32"/>
+      <c r="A46" s="30"/>
+      <c r="B46" s="30"/>
+      <c r="C46" s="30"/>
+      <c r="D46" s="30"/>
+      <c r="E46" s="30"/>
+      <c r="F46" s="30"/>
+      <c r="G46" s="30"/>
       <c r="H46" s="13"/>
       <c r="L46" s="13"/>
       <c r="O46" s="13"/>
@@ -2247,13 +2247,13 @@
       <c r="AD46" s="14"/>
     </row>
     <row r="47" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A47" s="32"/>
-      <c r="B47" s="32"/>
-      <c r="C47" s="32"/>
-      <c r="D47" s="32"/>
-      <c r="E47" s="32"/>
-      <c r="F47" s="32"/>
-      <c r="G47" s="32"/>
+      <c r="A47" s="30"/>
+      <c r="B47" s="30"/>
+      <c r="C47" s="30"/>
+      <c r="D47" s="30"/>
+      <c r="E47" s="30"/>
+      <c r="F47" s="30"/>
+      <c r="G47" s="30"/>
       <c r="H47" s="13"/>
       <c r="L47" s="13"/>
       <c r="O47" s="13"/>
@@ -2264,13 +2264,13 @@
       <c r="AD47" s="14"/>
     </row>
     <row r="48" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A48" s="32"/>
-      <c r="B48" s="32"/>
-      <c r="C48" s="32"/>
-      <c r="D48" s="32"/>
-      <c r="E48" s="32"/>
-      <c r="F48" s="32"/>
-      <c r="G48" s="32"/>
+      <c r="A48" s="30"/>
+      <c r="B48" s="30"/>
+      <c r="C48" s="30"/>
+      <c r="D48" s="30"/>
+      <c r="E48" s="30"/>
+      <c r="F48" s="30"/>
+      <c r="G48" s="30"/>
       <c r="H48" s="13"/>
       <c r="L48" s="13"/>
       <c r="O48" s="13"/>
@@ -2281,11 +2281,11 @@
       <c r="AD48" s="14"/>
     </row>
     <row r="49" spans="2:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B49" s="32"/>
-      <c r="C49" s="32"/>
-      <c r="D49" s="32"/>
-      <c r="E49" s="32"/>
-      <c r="F49" s="32"/>
+      <c r="B49" s="30"/>
+      <c r="C49" s="30"/>
+      <c r="D49" s="30"/>
+      <c r="E49" s="30"/>
+      <c r="F49" s="30"/>
       <c r="H49" s="13"/>
       <c r="L49" s="13"/>
       <c r="O49" s="13"/>
@@ -6237,16 +6237,16 @@
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="C18:F18"/>
+    <mergeCell ref="C19:F19"/>
+    <mergeCell ref="B13:F13"/>
+    <mergeCell ref="C16:F16"/>
+    <mergeCell ref="B12:F12"/>
     <mergeCell ref="H1:K1"/>
     <mergeCell ref="L1:O1"/>
     <mergeCell ref="B1:F5"/>
     <mergeCell ref="B9:F9"/>
     <mergeCell ref="C17:F17"/>
-    <mergeCell ref="C18:F18"/>
-    <mergeCell ref="C19:F19"/>
-    <mergeCell ref="B13:F13"/>
-    <mergeCell ref="C16:F16"/>
-    <mergeCell ref="B12:F12"/>
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="B13" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>

</xml_diff>